<commit_message>
changes on some graphics sizes and gcis
</commit_message>
<xml_diff>
--- a/err.xlsx
+++ b/err.xlsx
@@ -507,705 +507,705 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>beta_zero_gci_mix1</t>
+          <t>keff_gci_mix2</t>
         </is>
       </c>
       <c r="B4" t="n">
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0.012356823745043</v>
+        <v>0.001251305095458049</v>
       </c>
       <c r="D4" t="n">
-        <v>0.007275828836558774</v>
+        <v>0.0004673097490064522</v>
       </c>
       <c r="E4" t="n">
-        <v>0.002888785474750865</v>
+        <v>0.001968743137903417</v>
       </c>
       <c r="F4" t="n">
-        <v>0.01140375067530228</v>
+        <v>0.001795835112707919</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>beta_zero_sd_mix1</t>
+          <t>keff_sd_mix2</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.00114</v>
+        <v>9.000000000000001e-05</v>
       </c>
       <c r="C5" t="n">
-        <v>0.00313</v>
+        <v>9.1e-05</v>
       </c>
       <c r="D5" t="n">
-        <v>0.00323</v>
+        <v>9.000000000000001e-05</v>
       </c>
       <c r="E5" t="n">
-        <v>0.00322</v>
+        <v>9.3e-05</v>
       </c>
       <c r="F5" t="n">
-        <v>0.00307</v>
+        <v>9.2e-05</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>beta_eff_gci_mix1</t>
+          <t>beta_zero_gci_mix1</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>0.05431646503365661</v>
+        <v>0.012356823745043</v>
       </c>
       <c r="D6" t="n">
-        <v>0.006449417504386067</v>
+        <v>0.007275828836558774</v>
       </c>
       <c r="E6" t="n">
-        <v>0.06878545512544382</v>
+        <v>0.002888785474750865</v>
       </c>
       <c r="F6" t="n">
-        <v>0.00748802325035749</v>
+        <v>0.01140375067530228</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>beta_eff_sd_mix1</t>
+          <t>beta_zero_sd_mix1</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.00693</v>
+        <v>0.00114</v>
       </c>
       <c r="C7" t="n">
-        <v>0.01942</v>
+        <v>0.00313</v>
       </c>
       <c r="D7" t="n">
-        <v>0.01871</v>
+        <v>0.00323</v>
       </c>
       <c r="E7" t="n">
-        <v>0.01942</v>
+        <v>0.00322</v>
       </c>
       <c r="F7" t="n">
-        <v>0.01952</v>
+        <v>0.00307</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>gen_time_gci_mix1</t>
+          <t>beta_zero_gci_mix2</t>
         </is>
       </c>
       <c r="B8" t="n">
         <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0162582568209311</v>
+        <v>0.007721803763641467</v>
       </c>
       <c r="D8" t="n">
-        <v>0.01912165934522041</v>
+        <v>0.00595633289763957</v>
       </c>
       <c r="E8" t="n">
-        <v>0.0007683792095229297</v>
+        <v>0.001723749259314246</v>
       </c>
       <c r="F8" t="n">
-        <v>0.1174617310665487</v>
+        <v>0.0009696061362008852</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>gen_time_sd_mix1</t>
+          <t>beta_zero_sd_mix2</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.0005999999999999999</v>
+        <v>0.00114</v>
       </c>
       <c r="C9" t="n">
-        <v>0.00209</v>
+        <v>0.00113</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0019</v>
+        <v>0.00113</v>
       </c>
       <c r="E9" t="n">
-        <v>0.00181</v>
+        <v>0.00114</v>
       </c>
       <c r="F9" t="n">
-        <v>0.00233</v>
+        <v>0.00112</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>keff_doppler_gci_mix1</t>
+          <t>beta_eff_gci_mix1</t>
         </is>
       </c>
       <c r="B10" t="n">
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0002186611785883395</v>
+        <v>0.05431646503365661</v>
       </c>
       <c r="D10" t="n">
-        <v>4.764643563041015e-05</v>
+        <v>0.006449417504386067</v>
       </c>
       <c r="E10" t="n">
-        <v>0.001378251479336209</v>
+        <v>0.06878545512544382</v>
       </c>
       <c r="F10" t="n">
-        <v>0.02062956230704849</v>
+        <v>0.00748802325035749</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>keff_doppler_sd_mix1</t>
+          <t>beta_eff_sd_mix1</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>8.3e-05</v>
+        <v>0.00693</v>
       </c>
       <c r="C11" t="n">
-        <v>8.3e-05</v>
+        <v>0.01942</v>
       </c>
       <c r="D11" t="n">
-        <v>8.2e-05</v>
+        <v>0.01871</v>
       </c>
       <c r="E11" t="n">
-        <v>8.4e-05</v>
+        <v>0.01942</v>
       </c>
       <c r="F11" t="n">
-        <v>8.3e-05</v>
+        <v>0.01952</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>keff_rho_gci_mix1</t>
+          <t>beta_eff_gci_mix2</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>0.0002652668131179046</v>
+        <v>0.02123126350841696</v>
       </c>
       <c r="D12" t="n">
-        <v>0.0002582448264971674</v>
+        <v>0.01123907685846045</v>
       </c>
       <c r="E12" t="n">
-        <v>0.001107554278286199</v>
+        <v>0.0007271727047324961</v>
       </c>
       <c r="F12" t="n">
-        <v>0.02129224192389709</v>
+        <v>0.003959469479525302</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>keff_rho_sd_mix1</t>
+          <t>beta_eff_sd_mix2</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>8.2e-05</v>
+        <v>0.007979999999999999</v>
       </c>
       <c r="C13" t="n">
-        <v>8.6e-05</v>
+        <v>0.008030000000000001</v>
       </c>
       <c r="D13" t="n">
-        <v>8.000000000000001e-05</v>
+        <v>0.00808</v>
       </c>
       <c r="E13" t="n">
-        <v>8.3e-05</v>
+        <v>0.008070000000000001</v>
       </c>
       <c r="F13" t="n">
-        <v>8.1e-05</v>
+        <v>0.00796</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>doppler_coef_gci_mix1</t>
+          <t>gen_time_gci_mix1</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>0.01377747880554868</v>
+        <v>0.0162582568209311</v>
       </c>
       <c r="D14" t="n">
-        <v>0.06416629423091381</v>
+        <v>0.01912165934522041</v>
       </c>
       <c r="E14" t="n">
-        <v>0.02082958374887434</v>
+        <v>0.0007683792095229297</v>
       </c>
       <c r="F14" t="n">
-        <v>1.213724946892039</v>
+        <v>0.1174617310665487</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>doppler_coef_sd_mix1</t>
+          <t>gen_time_sd_mix1</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-3.333333333333324e-09</v>
+        <v>0.0005999999999999999</v>
       </c>
       <c r="C15" t="n">
-        <v>-4.566666666666668e-07</v>
+        <v>0.00209</v>
       </c>
       <c r="D15" t="n">
-        <v>-5.6e-07</v>
+        <v>0.0019</v>
       </c>
       <c r="E15" t="n">
-        <v>-5.2e-07</v>
+        <v>0.00181</v>
       </c>
       <c r="F15" t="n">
-        <v>-5.233333333333334e-07</v>
+        <v>0.00233</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>rho_coef_gci_mix1</t>
+          <t>gen_time_gci_mix2</t>
         </is>
       </c>
       <c r="B16" t="n">
         <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>0.02145773515459828</v>
+        <v>0.005859259291708343</v>
       </c>
       <c r="D16" t="n">
-        <v>0.2091682951873849</v>
+        <v>0.006590974517311554</v>
       </c>
       <c r="E16" t="n">
-        <v>0.01660005019501339</v>
+        <v>0.0004130789716054473</v>
       </c>
       <c r="F16" t="n">
-        <v>3.027576543045785</v>
+        <v>0.008394926785202459</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>rho_coef_sd_mix1</t>
+          <t>gen_time_sd_mix2</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0</v>
+        <v>0.00069</v>
       </c>
       <c r="C17" t="n">
-        <v>-5.826086956521739e-07</v>
+        <v>0.00076</v>
       </c>
       <c r="D17" t="n">
-        <v>-7.391304347826088e-07</v>
+        <v>0.00077</v>
       </c>
       <c r="E17" t="n">
-        <v>-6.82608695652174e-07</v>
+        <v>0.00084</v>
       </c>
       <c r="F17" t="n">
-        <v>-6.91304347826087e-07</v>
+        <v>0.00078</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>feedback_coef_gci_mix1</t>
+          <t>keff_doppler_gci_mix1</t>
         </is>
       </c>
       <c r="B18" t="n">
         <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>0.01652920593785676</v>
+        <v>0.0002186611785883395</v>
       </c>
       <c r="D18" t="n">
-        <v>0.116247944581917</v>
+        <v>4.764643563041015e-05</v>
       </c>
       <c r="E18" t="n">
-        <v>0.01934179399893252</v>
+        <v>0.001378251479336209</v>
       </c>
       <c r="F18" t="n">
-        <v>1.852638937661776</v>
+        <v>0.02062956230704849</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>feedback_coef_sd_mix1</t>
+          <t>keff_doppler_sd_mix1</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-3.333333333333324e-09</v>
+        <v>8.3e-05</v>
       </c>
       <c r="C19" t="n">
-        <v>-1.039275362318841e-06</v>
+        <v>8.3e-05</v>
       </c>
       <c r="D19" t="n">
-        <v>-1.299130434782609e-06</v>
+        <v>8.2e-05</v>
       </c>
       <c r="E19" t="n">
-        <v>-1.202608695652174e-06</v>
+        <v>8.4e-05</v>
       </c>
       <c r="F19" t="n">
-        <v>-1.21463768115942e-06</v>
+        <v>8.3e-05</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>keff_gci_mix2</t>
+          <t>keff_doppler_gci_mix2</t>
         </is>
       </c>
       <c r="B20" t="n">
         <v>0</v>
       </c>
       <c r="C20" t="n">
-        <v>0.001251305095458049</v>
+        <v>0.0008480837198011987</v>
       </c>
       <c r="D20" t="n">
-        <v>0.0004673097490064522</v>
+        <v>0.0008759721603055198</v>
       </c>
       <c r="E20" t="n">
-        <v>0.001968743137903417</v>
+        <v>0.0008285389282314645</v>
       </c>
       <c r="F20" t="n">
-        <v>0.001795835112707919</v>
+        <v>0.0001879418990048101</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>keff_sd_mix2</t>
+          <t>keff_doppler_sd_mix2</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>9.000000000000001e-05</v>
+        <v>8.899999999999999e-05</v>
       </c>
       <c r="C21" t="n">
-        <v>9.1e-05</v>
+        <v>9.399999999999999e-05</v>
       </c>
       <c r="D21" t="n">
-        <v>9.000000000000001e-05</v>
+        <v>9.3e-05</v>
       </c>
       <c r="E21" t="n">
+        <v>9.2e-05</v>
+      </c>
+      <c r="F21" t="n">
         <v>9.3e-05</v>
-      </c>
-      <c r="F21" t="n">
-        <v>9.2e-05</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>beta_zero_gci_mix2</t>
+          <t>keff_rho_gci_mix1</t>
         </is>
       </c>
       <c r="B22" t="n">
         <v>0</v>
       </c>
       <c r="C22" t="n">
-        <v>0.007721803763641467</v>
+        <v>0.0002652668131179046</v>
       </c>
       <c r="D22" t="n">
-        <v>0.00595633289763957</v>
+        <v>0.0002582448264971674</v>
       </c>
       <c r="E22" t="n">
-        <v>0.001723749259314246</v>
+        <v>0.001107554278286199</v>
       </c>
       <c r="F22" t="n">
-        <v>0.0009696061362008852</v>
+        <v>0.02129224192389709</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>beta_zero_sd_mix2</t>
+          <t>keff_rho_sd_mix1</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.00114</v>
+        <v>8.2e-05</v>
       </c>
       <c r="C23" t="n">
-        <v>0.00113</v>
+        <v>8.6e-05</v>
       </c>
       <c r="D23" t="n">
-        <v>0.00113</v>
+        <v>8.000000000000001e-05</v>
       </c>
       <c r="E23" t="n">
-        <v>0.00114</v>
+        <v>8.3e-05</v>
       </c>
       <c r="F23" t="n">
-        <v>0.00112</v>
+        <v>8.1e-05</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>beta_eff_gci_mix2</t>
+          <t>keff_rho_gci_mix2</t>
         </is>
       </c>
       <c r="B24" t="n">
         <v>0</v>
       </c>
       <c r="C24" t="n">
-        <v>0.02123126350841696</v>
+        <v>0.0003314545986762816</v>
       </c>
       <c r="D24" t="n">
-        <v>0.01123907685846045</v>
+        <v>2.037126087321999e-05</v>
       </c>
       <c r="E24" t="n">
-        <v>0.0007271727047324961</v>
+        <v>0.002449479221107563</v>
       </c>
       <c r="F24" t="n">
-        <v>0.003959469479525302</v>
+        <v>0.001119182988469765</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>beta_eff_sd_mix2</t>
+          <t>keff_rho_sd_mix2</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.007979999999999999</v>
+        <v>8.899999999999999e-05</v>
       </c>
       <c r="C25" t="n">
-        <v>0.008030000000000001</v>
+        <v>9.2e-05</v>
       </c>
       <c r="D25" t="n">
-        <v>0.00808</v>
+        <v>9.2e-05</v>
       </c>
       <c r="E25" t="n">
-        <v>0.008070000000000001</v>
+        <v>9.2e-05</v>
       </c>
       <c r="F25" t="n">
-        <v>0.00796</v>
+        <v>9.000000000000001e-05</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>gen_time_gci_mix2</t>
+          <t>doppler_coef_gci_mix1</t>
         </is>
       </c>
       <c r="B26" t="n">
         <v>0</v>
       </c>
       <c r="C26" t="n">
-        <v>0.005859259291708343</v>
+        <v>0.01377747880554868</v>
       </c>
       <c r="D26" t="n">
-        <v>0.006590974517311554</v>
+        <v>0.06416629423091381</v>
       </c>
       <c r="E26" t="n">
-        <v>0.0004130789716054473</v>
+        <v>0.02082958374887434</v>
       </c>
       <c r="F26" t="n">
-        <v>0.008394926785202459</v>
+        <v>1.213724946892039</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>gen_time_sd_mix2</t>
+          <t>doppler_coef_sd_mix1</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.00069</v>
+        <v>-3.333333333333324e-09</v>
       </c>
       <c r="C27" t="n">
-        <v>0.00076</v>
+        <v>-4.566666666666668e-07</v>
       </c>
       <c r="D27" t="n">
-        <v>0.00077</v>
+        <v>-5.6e-07</v>
       </c>
       <c r="E27" t="n">
-        <v>0.00084</v>
+        <v>-5.2e-07</v>
       </c>
       <c r="F27" t="n">
-        <v>0.00078</v>
+        <v>-5.233333333333334e-07</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>keff_doppler_gci_mix2</t>
+          <t>doppler_coef_gci_mix2</t>
         </is>
       </c>
       <c r="B28" t="n">
         <v>0</v>
       </c>
       <c r="C28" t="n">
-        <v>0.0008480837198011987</v>
+        <v>0.1428452689797494</v>
       </c>
       <c r="D28" t="n">
-        <v>0.0008759721603055198</v>
+        <v>0.005796285605458215</v>
       </c>
       <c r="E28" t="n">
-        <v>0.0008285389282314645</v>
+        <v>0.03376161593035037</v>
       </c>
       <c r="F28" t="n">
-        <v>0.0001879418990048101</v>
+        <v>0.150882472274823</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>keff_doppler_sd_mix2</t>
+          <t>doppler_coef_sd_mix2</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>8.899999999999999e-05</v>
+        <v>-3.333333333333369e-09</v>
       </c>
       <c r="C29" t="n">
-        <v>9.399999999999999e-05</v>
+        <v>-9.999999999999972e-09</v>
       </c>
       <c r="D29" t="n">
-        <v>9.3e-05</v>
+        <v>-9.999999999999972e-09</v>
       </c>
       <c r="E29" t="n">
-        <v>9.2e-05</v>
+        <v>-3.333333333333324e-09</v>
       </c>
       <c r="F29" t="n">
-        <v>9.3e-05</v>
+        <v>-3.333333333333324e-09</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>keff_rho_gci_mix2</t>
+          <t>rho_coef_gci_mix1</t>
         </is>
       </c>
       <c r="B30" t="n">
         <v>0</v>
       </c>
       <c r="C30" t="n">
-        <v>0.0003314545986762816</v>
+        <v>0.02145773515459828</v>
       </c>
       <c r="D30" t="n">
-        <v>2.037126087321999e-05</v>
+        <v>0.2091682951873849</v>
       </c>
       <c r="E30" t="n">
-        <v>0.002449479221107563</v>
+        <v>0.01660005019501339</v>
       </c>
       <c r="F30" t="n">
-        <v>0.001119182988469765</v>
+        <v>3.027576543045785</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>keff_rho_sd_mix2</t>
+          <t>rho_coef_sd_mix1</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>8.899999999999999e-05</v>
+        <v>-0</v>
       </c>
       <c r="C31" t="n">
-        <v>9.2e-05</v>
+        <v>-5.826086956521739e-07</v>
       </c>
       <c r="D31" t="n">
-        <v>9.2e-05</v>
+        <v>-7.391304347826088e-07</v>
       </c>
       <c r="E31" t="n">
-        <v>9.2e-05</v>
+        <v>-6.82608695652174e-07</v>
       </c>
       <c r="F31" t="n">
-        <v>9.000000000000001e-05</v>
+        <v>-6.91304347826087e-07</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>doppler_coef_gci_mix2</t>
+          <t>rho_coef_gci_mix2</t>
         </is>
       </c>
       <c r="B32" t="n">
         <v>0</v>
       </c>
       <c r="C32" t="n">
-        <v>0.1428452689797494</v>
+        <v>0.696793693642128</v>
       </c>
       <c r="D32" t="n">
-        <v>0.005796285605458215</v>
+        <v>0.4220551378444497</v>
       </c>
       <c r="E32" t="n">
-        <v>0.03376161593035037</v>
+        <v>0.1991794983008728</v>
       </c>
       <c r="F32" t="n">
-        <v>0.150882472274823</v>
+        <v>0.1565849410502993</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>doppler_coef_sd_mix2</t>
+          <t>rho_coef_sd_mix2</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>-3.333333333333369e-09</v>
+        <v>-4.347826086956569e-09</v>
       </c>
       <c r="C33" t="n">
-        <v>-9.999999999999972e-09</v>
+        <v>-4.347826086956509e-09</v>
       </c>
       <c r="D33" t="n">
-        <v>-9.999999999999972e-09</v>
+        <v>-8.695652173913019e-09</v>
       </c>
       <c r="E33" t="n">
-        <v>-3.333333333333324e-09</v>
+        <v>-4.347826086956509e-09</v>
       </c>
       <c r="F33" t="n">
-        <v>-3.333333333333324e-09</v>
+        <v>-8.695652173913019e-09</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>rho_coef_gci_mix2</t>
+          <t>feedback_coef_gci_mix1</t>
         </is>
       </c>
       <c r="B34" t="n">
         <v>0</v>
       </c>
       <c r="C34" t="n">
-        <v>0.696793693642128</v>
+        <v>0.01652920593785676</v>
       </c>
       <c r="D34" t="n">
-        <v>0.4220551378444497</v>
+        <v>0.116247944581917</v>
       </c>
       <c r="E34" t="n">
-        <v>0.1991794983008728</v>
+        <v>0.01934179399893252</v>
       </c>
       <c r="F34" t="n">
-        <v>0.1565849410502993</v>
+        <v>1.852638937661776</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>rho_coef_sd_mix2</t>
+          <t>feedback_coef_sd_mix1</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>-4.347826086956569e-09</v>
+        <v>-3.333333333333324e-09</v>
       </c>
       <c r="C35" t="n">
-        <v>-4.347826086956509e-09</v>
+        <v>-1.039275362318841e-06</v>
       </c>
       <c r="D35" t="n">
-        <v>-8.695652173913019e-09</v>
+        <v>-1.299130434782609e-06</v>
       </c>
       <c r="E35" t="n">
-        <v>-4.347826086956509e-09</v>
+        <v>-1.202608695652174e-06</v>
       </c>
       <c r="F35" t="n">
-        <v>-8.695652173913019e-09</v>
+        <v>-1.21463768115942e-06</v>
       </c>
     </row>
     <row r="36">

</xml_diff>